<commit_message>
lagadi burndown-baetti vid timum
</commit_message>
<xml_diff>
--- a/stada.xlsx
+++ b/stada.xlsx
@@ -752,46 +752,46 @@
                   <c:v>3210</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3210</c:v>
+                  <c:v>3130</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3210</c:v>
+                  <c:v>3130</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3210</c:v>
+                  <c:v>2950</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3210</c:v>
+                  <c:v>2890</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3210</c:v>
+                  <c:v>2530</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3210</c:v>
+                  <c:v>2110</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3210</c:v>
+                  <c:v>1630</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3210</c:v>
+                  <c:v>1630</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3210</c:v>
+                  <c:v>1630</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3210</c:v>
+                  <c:v>1630</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3210</c:v>
+                  <c:v>1630</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3210</c:v>
+                  <c:v>1630</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3210</c:v>
+                  <c:v>1630</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3210</c:v>
+                  <c:v>1630</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -808,11 +808,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="166116352"/>
-        <c:axId val="166609664"/>
+        <c:axId val="173530112"/>
+        <c:axId val="174011136"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="166116352"/>
+        <c:axId val="173530112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -822,14 +822,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166609664"/>
+        <c:crossAx val="174011136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="166609664"/>
+        <c:axId val="174011136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,7 +845,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="166116352"/>
+        <c:crossAx val="173530112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1241,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,10 +1326,10 @@
       </c>
       <c r="H3" s="6">
         <f>H2-I3</f>
-        <v>3210</v>
+        <v>3130</v>
       </c>
       <c r="I3" s="6">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J3" s="5">
         <v>41669</v>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="H4" s="6">
         <f t="shared" ref="H4:H15" si="0">H3-I4</f>
-        <v>3210</v>
+        <v>3130</v>
       </c>
       <c r="I4" s="6">
         <v>0</v>
@@ -1390,10 +1390,10 @@
       </c>
       <c r="H5" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>2950</v>
       </c>
       <c r="I5" s="6">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="J5" s="5">
         <v>41671</v>
@@ -1422,10 +1422,10 @@
       </c>
       <c r="H6" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>2890</v>
       </c>
       <c r="I6" s="6">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J6" s="5">
         <v>41672</v>
@@ -1454,10 +1454,10 @@
       </c>
       <c r="H7" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>2530</v>
       </c>
       <c r="I7" s="6">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="J7" s="5">
         <v>41673</v>
@@ -1474,10 +1474,10 @@
       </c>
       <c r="H8" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>2110</v>
       </c>
       <c r="I8" s="6">
-        <v>0</v>
+        <v>420</v>
       </c>
       <c r="J8" s="5">
         <v>41674</v>
@@ -1502,10 +1502,10 @@
       </c>
       <c r="H9" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>1630</v>
       </c>
       <c r="I9" s="6">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="J9" s="5">
         <v>41675</v>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="H10" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>1630</v>
       </c>
       <c r="I10" s="6">
         <v>0</v>
@@ -1558,7 +1558,7 @@
       </c>
       <c r="H11" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>1630</v>
       </c>
       <c r="I11" s="6">
         <v>0</v>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="H12" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>1630</v>
       </c>
       <c r="I12" s="6">
         <v>0</v>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="H13" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>1630</v>
       </c>
       <c r="I13" s="6">
         <v>0</v>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="H14" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>1630</v>
       </c>
       <c r="I14" s="6">
         <v>0</v>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="H15" s="6">
         <f t="shared" si="0"/>
-        <v>3210</v>
+        <v>1630</v>
       </c>
       <c r="I15" s="6">
         <v>0</v>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="H16" s="6">
         <f>H15-I16</f>
-        <v>3210</v>
+        <v>1630</v>
       </c>
       <c r="I16" s="6">
         <v>0</v>

</xml_diff>